<commit_message>
modified:   design_docs/Quest.xlsx 	modified:   fillin_player/fillin_player.py 	modified:   game_logic.py 	modified:   models/player.py 	modified:   routers/routes.py 	modified:   templates/logs.html 	modified:   test/test_alg.py 	new file:   test/test_invite.py 	modified:   timer.py
</commit_message>
<xml_diff>
--- a/design_docs/Quest.xlsx
+++ b/design_docs/Quest.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="38">
   <si>
     <t>id</t>
   </si>
@@ -122,6 +122,27 @@
   </si>
   <si>
     <t>[[1,90.8]]</t>
+  </si>
+  <si>
+    <t>被邀请人奖励</t>
+  </si>
+  <si>
+    <t>[[1,80]]</t>
+  </si>
+  <si>
+    <t>邀请人奖励</t>
+  </si>
+  <si>
+    <t>[[1,8]]</t>
+  </si>
+  <si>
+    <t>邀请人父节点奖励</t>
+  </si>
+  <si>
+    <t>[[1,82]]</t>
+  </si>
+  <si>
+    <t>邀请人祖父节点奖励</t>
   </si>
 </sst>
 </file>
@@ -1079,10 +1100,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:I15"/>
+  <dimension ref="A1:I19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.1"/>
@@ -1115,7 +1136,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" ht="14.85" spans="1:9">
       <c r="A2" s="1">
         <v>101</v>
       </c>
@@ -1139,7 +1160,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" ht="14.85" spans="1:9">
       <c r="A3" s="1">
         <v>102</v>
       </c>
@@ -1163,7 +1184,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" ht="14.85" spans="1:9">
       <c r="A4" s="1">
         <v>103</v>
       </c>
@@ -1187,7 +1208,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" ht="14.85" spans="1:7">
       <c r="A5" s="1">
         <v>104</v>
       </c>
@@ -1208,7 +1229,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" ht="14.85" spans="1:7">
       <c r="A6" s="1">
         <v>105</v>
       </c>
@@ -1229,7 +1250,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" ht="14.85" spans="1:7">
       <c r="A7" s="1">
         <v>106</v>
       </c>
@@ -1250,7 +1271,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" ht="14.85" spans="1:7">
       <c r="A8" s="1">
         <v>107</v>
       </c>
@@ -1271,7 +1292,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" ht="14.85" spans="1:7">
       <c r="A9" s="1">
         <v>201</v>
       </c>
@@ -1292,7 +1313,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" ht="14.85" spans="1:7">
       <c r="A10" s="1">
         <v>202</v>
       </c>
@@ -1313,7 +1334,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" ht="14.85" spans="1:7">
       <c r="A11" s="1">
         <v>203</v>
       </c>
@@ -1334,7 +1355,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" ht="14.85" spans="1:7">
       <c r="A12" s="1">
         <v>204</v>
       </c>
@@ -1355,7 +1376,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:7">
+    <row r="13" ht="14.85" spans="1:7">
       <c r="A13" s="1">
         <v>205</v>
       </c>
@@ -1376,7 +1397,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:7">
+    <row r="14" ht="14.85" spans="1:7">
       <c r="A14" s="1">
         <v>206</v>
       </c>
@@ -1397,7 +1418,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:7">
+    <row r="15" ht="14.85" spans="1:7">
       <c r="A15">
         <v>301</v>
       </c>
@@ -1413,6 +1434,86 @@
       <c r="E15" s="2"/>
       <c r="G15">
         <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7">
+      <c r="A16">
+        <v>4001</v>
+      </c>
+      <c r="B16">
+        <v>1</v>
+      </c>
+      <c r="C16">
+        <v>4</v>
+      </c>
+      <c r="D16" t="s">
+        <v>7</v>
+      </c>
+      <c r="F16" t="s">
+        <v>31</v>
+      </c>
+      <c r="G16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7">
+      <c r="A17">
+        <v>4002</v>
+      </c>
+      <c r="B17">
+        <v>1</v>
+      </c>
+      <c r="C17">
+        <v>4</v>
+      </c>
+      <c r="D17" t="s">
+        <v>32</v>
+      </c>
+      <c r="F17" t="s">
+        <v>33</v>
+      </c>
+      <c r="G17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7">
+      <c r="A18">
+        <v>4003</v>
+      </c>
+      <c r="B18">
+        <v>1</v>
+      </c>
+      <c r="C18">
+        <v>4</v>
+      </c>
+      <c r="D18" t="s">
+        <v>34</v>
+      </c>
+      <c r="F18" t="s">
+        <v>35</v>
+      </c>
+      <c r="G18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7">
+      <c r="A19">
+        <v>4004</v>
+      </c>
+      <c r="B19">
+        <v>1</v>
+      </c>
+      <c r="C19">
+        <v>4</v>
+      </c>
+      <c r="D19" t="s">
+        <v>36</v>
+      </c>
+      <c r="F19" t="s">
+        <v>37</v>
+      </c>
+      <c r="G19">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>